<commit_message>
feat: first sparql query
</commit_message>
<xml_diff>
--- a/Backend/src/main/resources/sec_ontology_individuals.xlsx
+++ b/Backend/src/main/resources/sec_ontology_individuals.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FTN\Semantic Web\semantic-web\Backend\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20265" windowHeight="11610" activeTab="4"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="KnowledgeAreas" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="KnowledgeUnits" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="LearningOutcomes" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Courses" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="LearningResources" sheetId="5" r:id="rId8"/>
+    <sheet name="KnowledgeAreas" sheetId="1" r:id="rId1"/>
+    <sheet name="KnowledgeUnits" sheetId="2" r:id="rId2"/>
+    <sheet name="LearningOutcomes" sheetId="3" r:id="rId3"/>
+    <sheet name="Courses" sheetId="4" r:id="rId4"/>
+    <sheet name="LearningResources" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="621">
   <si>
     <t>AL</t>
   </si>
@@ -1868,34 +1876,51 @@
   </si>
   <si>
     <t>R-4</t>
+  </si>
+  <si>
+    <t>Clean Code</t>
+  </si>
+  <si>
+    <t>Introduction to C</t>
+  </si>
+  <si>
+    <t>Database Basics</t>
+  </si>
+  <si>
+    <t>Pragmatic Programmer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1905,54 +1930,43 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -2142,24 +2156,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="37.57"/>
-    <col customWidth="1" min="2" max="2" width="40.86"/>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2167,10 +2184,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2178,10 +2195,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2189,10 +2206,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2200,10 +2217,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2211,10 +2228,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>40.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2222,10 +2239,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2233,10 +2250,10 @@
         <v>13</v>
       </c>
       <c r="C7" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -2244,10 +2261,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -2255,10 +2272,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -2266,10 +2283,10 @@
         <v>19</v>
       </c>
       <c r="C10" s="1">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -2277,10 +2294,10 @@
         <v>21</v>
       </c>
       <c r="C11" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -2288,10 +2305,10 @@
         <v>23</v>
       </c>
       <c r="C12" s="1">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -2299,10 +2316,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="1">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -2310,10 +2327,10 @@
         <v>27</v>
       </c>
       <c r="C14" s="1">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -2321,10 +2338,10 @@
         <v>29</v>
       </c>
       <c r="C15" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -2332,29 +2349,30 @@
         <v>31</v>
       </c>
       <c r="C16" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="58.43"/>
-    <col customWidth="1" min="3" max="3" width="60.57"/>
+    <col min="1" max="2" width="58.42578125" customWidth="1"/>
+    <col min="3" max="3" width="60.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2365,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -2376,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -2387,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -2398,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -2409,7 +2427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -2420,7 +2438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2431,7 +2449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2442,7 +2460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -2453,7 +2471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
@@ -2464,7 +2482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
@@ -2475,7 +2493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
@@ -2486,7 +2504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -2497,7 +2515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>58</v>
       </c>
@@ -2508,7 +2526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
@@ -2519,7 +2537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>62</v>
       </c>
@@ -2530,7 +2548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -2541,7 +2559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>66</v>
       </c>
@@ -2552,7 +2570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>68</v>
       </c>
@@ -2563,7 +2581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>70</v>
       </c>
@@ -2574,7 +2592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
@@ -2585,7 +2603,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>74</v>
       </c>
@@ -2596,7 +2614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
@@ -2607,7 +2625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -2618,7 +2636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -2629,7 +2647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
@@ -2640,7 +2658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>84</v>
       </c>
@@ -2651,7 +2669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>86</v>
       </c>
@@ -2662,7 +2680,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
@@ -2673,7 +2691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
@@ -2684,7 +2702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>92</v>
       </c>
@@ -2695,7 +2713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
@@ -2706,7 +2724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>96</v>
       </c>
@@ -2717,7 +2735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>98</v>
       </c>
@@ -2728,7 +2746,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
@@ -2739,7 +2757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>102</v>
       </c>
@@ -2750,7 +2768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -2761,7 +2779,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>106</v>
       </c>
@@ -2772,7 +2790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>108</v>
       </c>
@@ -2783,7 +2801,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>110</v>
       </c>
@@ -2794,7 +2812,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
@@ -2805,7 +2823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>114</v>
       </c>
@@ -2816,7 +2834,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>116</v>
       </c>
@@ -2827,7 +2845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>118</v>
       </c>
@@ -2838,7 +2856,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>120</v>
       </c>
@@ -2849,7 +2867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>122</v>
       </c>
@@ -2860,7 +2878,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>124</v>
       </c>
@@ -2871,7 +2889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>126</v>
       </c>
@@ -2882,7 +2900,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>128</v>
       </c>
@@ -2893,7 +2911,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>130</v>
       </c>
@@ -2904,7 +2922,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>132</v>
       </c>
@@ -2915,7 +2933,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>134</v>
       </c>
@@ -2926,7 +2944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>136</v>
       </c>
@@ -2937,7 +2955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>138</v>
       </c>
@@ -2948,7 +2966,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>140</v>
       </c>
@@ -2959,7 +2977,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>142</v>
       </c>
@@ -2970,7 +2988,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>144</v>
       </c>
@@ -2981,7 +2999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>146</v>
       </c>
@@ -2992,7 +3010,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>148</v>
       </c>
@@ -3003,7 +3021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>150</v>
       </c>
@@ -3014,7 +3032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>152</v>
       </c>
@@ -3025,7 +3043,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>154</v>
       </c>
@@ -3036,7 +3054,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>156</v>
       </c>
@@ -3047,7 +3065,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>158</v>
       </c>
@@ -3059,26 +3077,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.29"/>
-    <col customWidth="1" min="2" max="2" width="94.29"/>
-    <col customWidth="1" min="3" max="3" width="28.29"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="94.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -3089,7 +3108,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>162</v>
       </c>
@@ -3100,7 +3119,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>164</v>
       </c>
@@ -3111,7 +3130,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>166</v>
       </c>
@@ -3122,7 +3141,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>168</v>
       </c>
@@ -3133,7 +3152,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>170</v>
       </c>
@@ -3144,7 +3163,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>172</v>
       </c>
@@ -3155,7 +3174,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>174</v>
       </c>
@@ -3166,7 +3185,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>176</v>
       </c>
@@ -3177,7 +3196,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>178</v>
       </c>
@@ -3188,7 +3207,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>180</v>
       </c>
@@ -3199,7 +3218,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>182</v>
       </c>
@@ -3210,7 +3229,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>184</v>
       </c>
@@ -3221,7 +3240,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>186</v>
       </c>
@@ -3232,7 +3251,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>188</v>
       </c>
@@ -3243,7 +3262,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>190</v>
       </c>
@@ -3254,7 +3273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>192</v>
       </c>
@@ -3265,7 +3284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>194</v>
       </c>
@@ -3276,7 +3295,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>196</v>
       </c>
@@ -3287,7 +3306,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>198</v>
       </c>
@@ -3298,7 +3317,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>200</v>
       </c>
@@ -3309,7 +3328,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>202</v>
       </c>
@@ -3320,7 +3339,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>204</v>
       </c>
@@ -3331,7 +3350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>206</v>
       </c>
@@ -3342,7 +3361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>208</v>
       </c>
@@ -3353,7 +3372,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>210</v>
       </c>
@@ -3364,7 +3383,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>212</v>
       </c>
@@ -3375,7 +3394,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>214</v>
       </c>
@@ -3386,7 +3405,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>216</v>
       </c>
@@ -3397,7 +3416,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>218</v>
       </c>
@@ -3408,7 +3427,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>220</v>
       </c>
@@ -3419,7 +3438,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>222</v>
       </c>
@@ -3430,7 +3449,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>224</v>
       </c>
@@ -3441,7 +3460,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>226</v>
       </c>
@@ -3452,7 +3471,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>228</v>
       </c>
@@ -3463,7 +3482,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>230</v>
       </c>
@@ -3474,7 +3493,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>232</v>
       </c>
@@ -3485,7 +3504,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>234</v>
       </c>
@@ -3496,7 +3515,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>236</v>
       </c>
@@ -3507,7 +3526,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>238</v>
       </c>
@@ -3518,7 +3537,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>240</v>
       </c>
@@ -3529,7 +3548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>242</v>
       </c>
@@ -3540,7 +3559,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>244</v>
       </c>
@@ -3551,7 +3570,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>246</v>
       </c>
@@ -3562,7 +3581,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>248</v>
       </c>
@@ -3573,7 +3592,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>250</v>
       </c>
@@ -3584,7 +3603,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>252</v>
       </c>
@@ -3595,7 +3614,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>254</v>
       </c>
@@ -3606,7 +3625,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>256</v>
       </c>
@@ -3617,7 +3636,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>258</v>
       </c>
@@ -3628,7 +3647,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>260</v>
       </c>
@@ -3639,7 +3658,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>262</v>
       </c>
@@ -3650,7 +3669,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>264</v>
       </c>
@@ -3661,7 +3680,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>266</v>
       </c>
@@ -3672,7 +3691,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>268</v>
       </c>
@@ -3683,7 +3702,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>270</v>
       </c>
@@ -3694,7 +3713,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>272</v>
       </c>
@@ -3705,7 +3724,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>274</v>
       </c>
@@ -3716,7 +3735,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>276</v>
       </c>
@@ -3727,7 +3746,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>278</v>
       </c>
@@ -3738,7 +3757,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>280</v>
       </c>
@@ -3749,7 +3768,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>282</v>
       </c>
@@ -3760,7 +3779,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>284</v>
       </c>
@@ -3771,7 +3790,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>286</v>
       </c>
@@ -3782,7 +3801,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>288</v>
       </c>
@@ -3793,7 +3812,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>290</v>
       </c>
@@ -3804,7 +3823,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>292</v>
       </c>
@@ -3815,7 +3834,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>294</v>
       </c>
@@ -3826,7 +3845,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>296</v>
       </c>
@@ -3837,7 +3856,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>298</v>
       </c>
@@ -3848,7 +3867,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>300</v>
       </c>
@@ -3859,7 +3878,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>302</v>
       </c>
@@ -3870,7 +3889,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>304</v>
       </c>
@@ -3881,7 +3900,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>306</v>
       </c>
@@ -3892,7 +3911,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>308</v>
       </c>
@@ -3903,7 +3922,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>310</v>
       </c>
@@ -3914,7 +3933,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>312</v>
       </c>
@@ -3925,7 +3944,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>314</v>
       </c>
@@ -3936,7 +3955,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>316</v>
       </c>
@@ -3947,7 +3966,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>318</v>
       </c>
@@ -3958,7 +3977,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>320</v>
       </c>
@@ -3969,7 +3988,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>322</v>
       </c>
@@ -3980,7 +3999,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>324</v>
       </c>
@@ -3991,7 +4010,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>326</v>
       </c>
@@ -4002,7 +4021,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>328</v>
       </c>
@@ -4013,7 +4032,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>330</v>
       </c>
@@ -4024,7 +4043,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>332</v>
       </c>
@@ -4035,7 +4054,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>334</v>
       </c>
@@ -4046,7 +4065,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>336</v>
       </c>
@@ -4057,7 +4076,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>338</v>
       </c>
@@ -4068,7 +4087,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>340</v>
       </c>
@@ -4079,7 +4098,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>342</v>
       </c>
@@ -4090,7 +4109,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>344</v>
       </c>
@@ -4101,7 +4120,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>346</v>
       </c>
@@ -4112,7 +4131,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>348</v>
       </c>
@@ -4123,7 +4142,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>350</v>
       </c>
@@ -4134,7 +4153,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>352</v>
       </c>
@@ -4145,7 +4164,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>354</v>
       </c>
@@ -4156,7 +4175,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>356</v>
       </c>
@@ -4167,7 +4186,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>358</v>
       </c>
@@ -4178,7 +4197,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>360</v>
       </c>
@@ -4189,7 +4208,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>362</v>
       </c>
@@ -4200,7 +4219,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>364</v>
       </c>
@@ -4211,7 +4230,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>366</v>
       </c>
@@ -4222,7 +4241,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>368</v>
       </c>
@@ -4233,7 +4252,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>370</v>
       </c>
@@ -4244,7 +4263,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>372</v>
       </c>
@@ -4255,7 +4274,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>374</v>
       </c>
@@ -4266,7 +4285,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>376</v>
       </c>
@@ -4277,7 +4296,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>378</v>
       </c>
@@ -4288,7 +4307,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>380</v>
       </c>
@@ -4299,7 +4318,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>382</v>
       </c>
@@ -4310,7 +4329,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>384</v>
       </c>
@@ -4321,7 +4340,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>386</v>
       </c>
@@ -4332,7 +4351,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>388</v>
       </c>
@@ -4343,7 +4362,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>390</v>
       </c>
@@ -4354,7 +4373,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>392</v>
       </c>
@@ -4365,7 +4384,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>394</v>
       </c>
@@ -4376,7 +4395,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>396</v>
       </c>
@@ -4387,7 +4406,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>398</v>
       </c>
@@ -4398,7 +4417,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>400</v>
       </c>
@@ -4409,7 +4428,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>402</v>
       </c>
@@ -4420,7 +4439,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>404</v>
       </c>
@@ -4431,7 +4450,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>406</v>
       </c>
@@ -4442,7 +4461,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>408</v>
       </c>
@@ -4453,7 +4472,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>410</v>
       </c>
@@ -4464,7 +4483,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>412</v>
       </c>
@@ -4475,7 +4494,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>414</v>
       </c>
@@ -4486,7 +4505,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>416</v>
       </c>
@@ -4497,7 +4516,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>418</v>
       </c>
@@ -4508,7 +4527,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>420</v>
       </c>
@@ -4519,7 +4538,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>422</v>
       </c>
@@ -4530,7 +4549,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>424</v>
       </c>
@@ -4541,7 +4560,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>426</v>
       </c>
@@ -4552,7 +4571,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>428</v>
       </c>
@@ -4563,7 +4582,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>430</v>
       </c>
@@ -4574,7 +4593,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>432</v>
       </c>
@@ -4585,7 +4604,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>434</v>
       </c>
@@ -4596,7 +4615,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>436</v>
       </c>
@@ -4607,7 +4626,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>438</v>
       </c>
@@ -4618,7 +4637,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>440</v>
       </c>
@@ -4629,7 +4648,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>442</v>
       </c>
@@ -4640,7 +4659,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>444</v>
       </c>
@@ -4651,7 +4670,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>446</v>
       </c>
@@ -4662,7 +4681,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>448</v>
       </c>
@@ -4673,7 +4692,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>450</v>
       </c>
@@ -4684,7 +4703,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>452</v>
       </c>
@@ -4695,7 +4714,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>454</v>
       </c>
@@ -4706,7 +4725,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>456</v>
       </c>
@@ -4717,7 +4736,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>458</v>
       </c>
@@ -4728,7 +4747,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>460</v>
       </c>
@@ -4739,7 +4758,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>462</v>
       </c>
@@ -4750,7 +4769,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>464</v>
       </c>
@@ -4761,7 +4780,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>466</v>
       </c>
@@ -4772,7 +4791,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>468</v>
       </c>
@@ -4783,7 +4802,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>470</v>
       </c>
@@ -4794,7 +4813,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>472</v>
       </c>
@@ -4805,7 +4824,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>474</v>
       </c>
@@ -4816,7 +4835,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>476</v>
       </c>
@@ -4827,7 +4846,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>478</v>
       </c>
@@ -4838,7 +4857,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>480</v>
       </c>
@@ -4849,7 +4868,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>482</v>
       </c>
@@ -4860,7 +4879,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>484</v>
       </c>
@@ -4871,7 +4890,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>486</v>
       </c>
@@ -4882,7 +4901,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>488</v>
       </c>
@@ -4893,7 +4912,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>490</v>
       </c>
@@ -4904,7 +4923,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>492</v>
       </c>
@@ -4915,7 +4934,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>494</v>
       </c>
@@ -4926,7 +4945,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>496</v>
       </c>
@@ -4937,7 +4956,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>498</v>
       </c>
@@ -4948,7 +4967,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>500</v>
       </c>
@@ -4959,7 +4978,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>502</v>
       </c>
@@ -4970,7 +4989,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>504</v>
       </c>
@@ -4981,7 +5000,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>506</v>
       </c>
@@ -4992,7 +5011,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>508</v>
       </c>
@@ -5003,7 +5022,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>510</v>
       </c>
@@ -5014,7 +5033,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>512</v>
       </c>
@@ -5025,7 +5044,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>514</v>
       </c>
@@ -5036,7 +5055,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>516</v>
       </c>
@@ -5047,7 +5066,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>518</v>
       </c>
@@ -5058,7 +5077,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>520</v>
       </c>
@@ -5069,7 +5088,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>522</v>
       </c>
@@ -5080,7 +5099,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>524</v>
       </c>
@@ -5091,7 +5110,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>526</v>
       </c>
@@ -5102,7 +5121,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>528</v>
       </c>
@@ -5113,7 +5132,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>530</v>
       </c>
@@ -5124,7 +5143,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>532</v>
       </c>
@@ -5135,7 +5154,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>534</v>
       </c>
@@ -5146,7 +5165,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>536</v>
       </c>
@@ -5157,7 +5176,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>538</v>
       </c>
@@ -5168,7 +5187,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>540</v>
       </c>
@@ -5179,7 +5198,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>542</v>
       </c>
@@ -5190,7 +5209,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>544</v>
       </c>
@@ -5201,7 +5220,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>546</v>
       </c>
@@ -5212,7 +5231,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>548</v>
       </c>
@@ -5223,7 +5242,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>550</v>
       </c>
@@ -5234,7 +5253,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>552</v>
       </c>
@@ -5245,7 +5264,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>554</v>
       </c>
@@ -5256,7 +5275,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>556</v>
       </c>
@@ -5267,7 +5286,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>558</v>
       </c>
@@ -5278,7 +5297,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>560</v>
       </c>
@@ -5289,7 +5308,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>562</v>
       </c>
@@ -5300,7 +5319,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>564</v>
       </c>
@@ -5311,7 +5330,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>566</v>
       </c>
@@ -5322,7 +5341,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>568</v>
       </c>
@@ -5333,7 +5352,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>570</v>
       </c>
@@ -5344,7 +5363,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>572</v>
       </c>
@@ -5355,7 +5374,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>574</v>
       </c>
@@ -5366,7 +5385,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>576</v>
       </c>
@@ -5377,7 +5396,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>578</v>
       </c>
@@ -5388,7 +5407,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>580</v>
       </c>
@@ -5399,7 +5418,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>582</v>
       </c>
@@ -5410,7 +5429,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>584</v>
       </c>
@@ -5421,7 +5440,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>586</v>
       </c>
@@ -5433,25 +5452,26 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="50.57"/>
-    <col customWidth="1" min="3" max="3" width="80.43"/>
+    <col min="2" max="2" width="50.5703125" customWidth="1"/>
+    <col min="3" max="3" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>588</v>
       </c>
@@ -5462,16 +5482,16 @@
         <v>590</v>
       </c>
       <c r="D1" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>592</v>
       </c>
@@ -5482,16 +5502,16 @@
         <v>593</v>
       </c>
       <c r="D2" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>594</v>
       </c>
@@ -5502,16 +5522,16 @@
         <v>596</v>
       </c>
       <c r="D3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>598</v>
       </c>
@@ -5522,16 +5542,16 @@
         <v>600</v>
       </c>
       <c r="D4" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>602</v>
       </c>
@@ -5542,34 +5562,37 @@
         <v>604</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>601</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="57.43"/>
+    <col min="4" max="4" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>605</v>
       </c>
@@ -5583,13 +5606,16 @@
         <v>607</v>
       </c>
       <c r="E1" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="G1" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>609</v>
       </c>
@@ -5603,13 +5629,16 @@
         <v>610</v>
       </c>
       <c r="E2" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="G2" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>612</v>
       </c>
@@ -5623,13 +5652,16 @@
         <v>614</v>
       </c>
       <c r="E3" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>616</v>
       </c>
@@ -5643,13 +5675,16 @@
         <v>604</v>
       </c>
       <c r="E4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>615</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>620</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>